<commit_message>
Some Goal classes for Garrison (WIP)
</commit_message>
<xml_diff>
--- a/GOAP goals and actions.xlsx
+++ b/GOAP goals and actions.xlsx
@@ -4,8 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="23100" windowHeight="17445"/>
-    <workbookView xWindow="19200" yWindow="75" windowWidth="19200" windowHeight="17415" activeTab="2"/>
+    <workbookView xWindow="75" yWindow="300" windowWidth="14340" windowHeight="12015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -293,7 +292,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +323,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -337,13 +342,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -640,17 +646,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="62" customWidth="1"/>
     <col min="7" max="7" width="25.42578125" customWidth="1"/>
   </cols>
@@ -869,11 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A1:XFD1048576"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -900,7 +902,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" s="4" customFormat="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -908,7 +910,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" s="4" customFormat="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -948,7 +950,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" s="4" customFormat="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -956,7 +958,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" s="4" customFormat="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1032,6 +1034,7 @@
     <row r="49" s="4" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1040,9 +1043,6 @@
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="1">
-      <selection activeCell="B34" sqref="B34"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
New actions, worldState restructure and functions
</commit_message>
<xml_diff>
--- a/GOAP goals and actions.xlsx
+++ b/GOAP goals and actions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="300" windowWidth="14340" windowHeight="12015" activeTab="1"/>
+    <workbookView xWindow="75" yWindow="300" windowWidth="14340" windowHeight="12015" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="87">
   <si>
     <t>Garrison goal</t>
   </si>
@@ -647,7 +647,7 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="C17" sqref="C17:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1042,7 +1042,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1315,6 +1317,12 @@
       <c r="C36" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1">
       <c r="B37" s="1" t="s">

</xml_diff>